<commit_message>
(2017/12/16) ESTRUTURA DAS APOSTAS - POT ODDS
Faze inicial da planilha
estrutura do cenario das jogadas
pot odds dos jogadores
</commit_message>
<xml_diff>
--- a/Analista/Planinhas Execel/Analizador.xlsx
+++ b/Analista/Planinhas Execel/Analizador.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="19">
   <si>
     <t xml:space="preserve">RODADA</t>
   </si>
@@ -71,6 +71,12 @@
   </si>
   <si>
     <t xml:space="preserve">FLOP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TURN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RIVER</t>
   </si>
 </sst>
 </file>
@@ -170,10 +176,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L5"/>
+  <dimension ref="A1:L10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H5" activeCellId="0" sqref="H5"/>
+      <selection pane="topLeft" activeCell="L10" activeCellId="0" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -334,6 +340,256 @@
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
         <v>16</v>
+      </c>
+      <c r="B5" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>60</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G5" s="0" t="n">
+        <f aca="false">SUM(B5:F5)+G4</f>
+        <v>240</v>
+      </c>
+      <c r="H5" s="0" t="n">
+        <f aca="false">(B5*100)/(B5+G5)</f>
+        <v>11.1111111111111</v>
+      </c>
+      <c r="I5" s="0" t="n">
+        <f aca="false">(C5*100)/(C5+G5)</f>
+        <v>20</v>
+      </c>
+      <c r="J5" s="0" t="n">
+        <f aca="false">(D5*100)/(D5+G5)</f>
+        <v>0</v>
+      </c>
+      <c r="K5" s="0" t="n">
+        <f aca="false">(E5*100)/(E5+G5)</f>
+        <v>0</v>
+      </c>
+      <c r="L5" s="0" t="n">
+        <f aca="false">(F5*100)/(F5+G5)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B6" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="C6" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D6" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E6" s="0" t="n">
+        <v>60</v>
+      </c>
+      <c r="F6" s="0" t="n">
+        <v>60</v>
+      </c>
+      <c r="G6" s="0" t="n">
+        <f aca="false">SUM(B6:F6)+G5</f>
+        <v>390</v>
+      </c>
+      <c r="H6" s="0" t="n">
+        <f aca="false">(B6*100)/(B6+G6)</f>
+        <v>7.14285714285714</v>
+      </c>
+      <c r="I6" s="0" t="n">
+        <f aca="false">(C6*100)/(C6+G6)</f>
+        <v>0</v>
+      </c>
+      <c r="J6" s="0" t="n">
+        <f aca="false">(D6*100)/(D6+G6)</f>
+        <v>0</v>
+      </c>
+      <c r="K6" s="0" t="n">
+        <f aca="false">(E6*100)/(E6+G6)</f>
+        <v>13.3333333333333</v>
+      </c>
+      <c r="L6" s="0" t="n">
+        <f aca="false">(F6*100)/(F6+G6)</f>
+        <v>13.3333333333333</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="0" t="n">
+        <v>200</v>
+      </c>
+      <c r="C7" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D7" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E7" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="F7" s="0" t="n">
+        <v>150</v>
+      </c>
+      <c r="G7" s="0" t="n">
+        <f aca="false">SUM(B7:F7)+G6</f>
+        <v>840</v>
+      </c>
+      <c r="H7" s="0" t="n">
+        <f aca="false">(B7*100)/(B7+G7)</f>
+        <v>19.2307692307692</v>
+      </c>
+      <c r="I7" s="0" t="n">
+        <f aca="false">(C7*100)/(C7+G7)</f>
+        <v>0</v>
+      </c>
+      <c r="J7" s="0" t="n">
+        <f aca="false">(D7*100)/(D7+G7)</f>
+        <v>0</v>
+      </c>
+      <c r="K7" s="0" t="n">
+        <f aca="false">(E7*100)/(E7+G7)</f>
+        <v>10.6382978723404</v>
+      </c>
+      <c r="L7" s="0" t="n">
+        <f aca="false">(F7*100)/(F7+G7)</f>
+        <v>15.1515151515152</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B8" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C8" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D8" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E8" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="F8" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="G8" s="0" t="n">
+        <f aca="false">SUM(B8:F8)+G7</f>
+        <v>990</v>
+      </c>
+      <c r="H8" s="0" t="n">
+        <f aca="false">(B8*100)/(B8+G8)</f>
+        <v>0</v>
+      </c>
+      <c r="I8" s="0" t="n">
+        <f aca="false">(C8*100)/(C8+G8)</f>
+        <v>0</v>
+      </c>
+      <c r="J8" s="0" t="n">
+        <f aca="false">(D8*100)/(D8+G8)</f>
+        <v>0</v>
+      </c>
+      <c r="K8" s="0" t="n">
+        <f aca="false">(E8*100)/(E8+G8)</f>
+        <v>9.1743119266055</v>
+      </c>
+      <c r="L8" s="0" t="n">
+        <f aca="false">(F8*100)/(F8+G8)</f>
+        <v>4.80769230769231</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" s="0" t="n">
+        <v>200</v>
+      </c>
+      <c r="C9" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D9" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E9" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="F9" s="0" t="n">
+        <v>150</v>
+      </c>
+      <c r="G9" s="0" t="n">
+        <f aca="false">SUM(B9:F9)+G8</f>
+        <v>1390</v>
+      </c>
+      <c r="H9" s="0" t="n">
+        <f aca="false">(B9*100)/(B9+G9)</f>
+        <v>12.5786163522013</v>
+      </c>
+      <c r="I9" s="0" t="n">
+        <f aca="false">(C9*100)/(C9+G9)</f>
+        <v>0</v>
+      </c>
+      <c r="J9" s="0" t="n">
+        <f aca="false">(D9*100)/(D9+G9)</f>
+        <v>0</v>
+      </c>
+      <c r="K9" s="0" t="n">
+        <f aca="false">(E9*100)/(E9+G9)</f>
+        <v>3.47222222222222</v>
+      </c>
+      <c r="L9" s="0" t="n">
+        <f aca="false">(F9*100)/(F9+G9)</f>
+        <v>9.74025974025974</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B10" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C10" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D10" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E10" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F10" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="G10" s="0" t="n">
+        <f aca="false">SUM(B10:F10)+G9</f>
+        <v>1440</v>
+      </c>
+      <c r="H10" s="0" t="n">
+        <f aca="false">(B10*100)/(B10+G10)</f>
+        <v>0</v>
+      </c>
+      <c r="I10" s="0" t="n">
+        <f aca="false">(C10*100)/(C10+G10)</f>
+        <v>0</v>
+      </c>
+      <c r="J10" s="0" t="n">
+        <f aca="false">(D10*100)/(D10+G10)</f>
+        <v>0</v>
+      </c>
+      <c r="K10" s="0" t="n">
+        <f aca="false">(E10*100)/(E10+G10)</f>
+        <v>0</v>
+      </c>
+      <c r="L10" s="0" t="n">
+        <f aca="false">(F10*100)/(F10+G10)</f>
+        <v>3.35570469798658</v>
       </c>
     </row>
   </sheetData>

</xml_diff>